<commit_message>
adding points on map
</commit_message>
<xml_diff>
--- a/data/ids_cities_states.xlsx
+++ b/data/ids_cities_states.xlsx
@@ -1,36 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomcairns/Downloads/Classes/DS 4200/Final Project/s-l-project-urban-beekeeping-laboratory-1/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanliang/Ryan Liang/college/second yr/second sem/info visual/DS4200/project/s-l-project-urban-beekeeping-laboratory-1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5197C0-FB81-4146-949B-04C6E25F33D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322D62C5-AE1B-024C-B26F-0CC5C8AFD33A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32280" yWindow="3420" windowWidth="25600" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="217">
   <si>
     <t>Hive ID</t>
   </si>
@@ -605,12 +595,6 @@
     <t>Brookline</t>
   </si>
   <si>
-    <t>Eatham</t>
-  </si>
-  <si>
-    <t>Hignham</t>
-  </si>
-  <si>
     <t>Arlington</t>
   </si>
   <si>
@@ -641,9 +625,6 @@
     <t>Medfield</t>
   </si>
   <si>
-    <t>Subury</t>
-  </si>
-  <si>
     <t>Jeffersonville</t>
   </si>
   <si>
@@ -662,15 +643,9 @@
     <t>Andover</t>
   </si>
   <si>
-    <t>Billericka</t>
-  </si>
-  <si>
     <t>Belmont</t>
   </si>
   <si>
-    <t>Medfeild</t>
-  </si>
-  <si>
     <t>Newport</t>
   </si>
   <si>
@@ -687,6 +662,15 @@
   </si>
   <si>
     <t>Newton Center</t>
+  </si>
+  <si>
+    <t>Eastham</t>
+  </si>
+  <si>
+    <t>Hingham</t>
+  </si>
+  <si>
+    <t>Billerica</t>
   </si>
 </sst>
 </file>
@@ -1028,11 +1012,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117:XFD117"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1842,7 +1829,7 @@
         <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="C74" t="s">
         <v>124</v>
@@ -1864,7 +1851,7 @@
         <v>84</v>
       </c>
       <c r="B76" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="C76" t="s">
         <v>124</v>
@@ -1875,7 +1862,7 @@
         <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C77" t="s">
         <v>124</v>
@@ -1886,7 +1873,7 @@
         <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C78" t="s">
         <v>129</v>
@@ -1897,10 +1884,10 @@
         <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C79" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -1908,10 +1895,10 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C80" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
@@ -1919,10 +1906,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C81" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
@@ -1930,10 +1917,10 @@
         <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C82" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
@@ -1941,10 +1928,10 @@
         <v>77</v>
       </c>
       <c r="B83" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -1952,7 +1939,7 @@
         <v>76</v>
       </c>
       <c r="B84" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C84" t="s">
         <v>172</v>
@@ -1996,7 +1983,7 @@
         <v>75</v>
       </c>
       <c r="B88" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C88" t="s">
         <v>127</v>
@@ -2007,7 +1994,7 @@
         <v>74</v>
       </c>
       <c r="B89" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C89" t="s">
         <v>131</v>
@@ -2040,7 +2027,7 @@
         <v>71</v>
       </c>
       <c r="B92" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C92" t="s">
         <v>124</v>
@@ -2051,7 +2038,7 @@
         <v>70</v>
       </c>
       <c r="B93" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
       <c r="C93" t="s">
         <v>124</v>
@@ -2073,7 +2060,7 @@
         <v>68</v>
       </c>
       <c r="B95" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C95" t="s">
         <v>168</v>
@@ -2106,7 +2093,7 @@
         <v>65</v>
       </c>
       <c r="B98" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C98" t="s">
         <v>150</v>
@@ -2117,7 +2104,7 @@
         <v>64</v>
       </c>
       <c r="B99" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C99" t="s">
         <v>156</v>
@@ -2139,7 +2126,7 @@
         <v>62</v>
       </c>
       <c r="B101" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C101" t="s">
         <v>124</v>
@@ -2150,7 +2137,7 @@
         <v>61</v>
       </c>
       <c r="B102" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C102" t="s">
         <v>124</v>
@@ -2161,7 +2148,7 @@
         <v>60</v>
       </c>
       <c r="B103" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C103" t="s">
         <v>124</v>
@@ -2172,7 +2159,7 @@
         <v>59</v>
       </c>
       <c r="B104" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C104" t="s">
         <v>124</v>
@@ -2205,7 +2192,7 @@
         <v>56</v>
       </c>
       <c r="B107" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C107" t="s">
         <v>124</v>
@@ -2216,7 +2203,7 @@
         <v>55</v>
       </c>
       <c r="B108" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C108" t="s">
         <v>124</v>
@@ -2227,7 +2214,7 @@
         <v>54</v>
       </c>
       <c r="B109" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C109" t="s">
         <v>124</v>
@@ -2260,7 +2247,7 @@
         <v>51</v>
       </c>
       <c r="B112" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C112" t="s">
         <v>124</v>
@@ -2282,7 +2269,7 @@
         <v>49</v>
       </c>
       <c r="B114" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C114" t="s">
         <v>156</v>
@@ -2315,7 +2302,7 @@
         <v>46</v>
       </c>
       <c r="B117" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C117" t="s">
         <v>129</v>
@@ -2326,7 +2313,7 @@
         <v>45</v>
       </c>
       <c r="B118" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C118" t="s">
         <v>172</v>
@@ -2348,7 +2335,7 @@
         <v>43</v>
       </c>
       <c r="B120" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C120" t="s">
         <v>124</v>
@@ -2359,7 +2346,7 @@
         <v>42</v>
       </c>
       <c r="B121" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C121" t="s">
         <v>124</v>
@@ -2370,7 +2357,7 @@
         <v>41</v>
       </c>
       <c r="B122" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C122" t="s">
         <v>124</v>

</xml_diff>